<commit_message>
Updated MicroPython demo hex
</commit_message>
<xml_diff>
--- a/component_tracking_solderbit.xlsx
+++ b/component_tracking_solderbit.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10512"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aroneggens/Desktop/solderbit-gamepad/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7F7CB58-F8F7-E440-A16D-0AEC3B480D84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A71C4F4-0E75-004F-AD1A-FBC6AEE10513}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33900" windowHeight="16780" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="33900" windowHeight="16780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts stock" sheetId="1" r:id="rId1"/>
@@ -711,7 +711,9 @@
   </sheetPr>
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1183,8 +1185,8 @@
   </sheetPr>
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="A1:C11"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>